<commit_message>
Add Protect Powell in Brief
Adjustments to Combined PowellMead, Powell10-Year, Time to Dead Pool
</commit_message>
<xml_diff>
--- a/Powell10year/PowellBypass.xlsx
+++ b/Powell10year/PowellBypass.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCoding2\Powell10year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D2B7E9F-2FAA-4DA7-BFDA-6DC321C4BB7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7368A42-5A39-4740-A3CF-3FB528BA8B32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810" xr2:uid="{EA0F2C89-335D-4615-958E-53520B7AFBE6}"/>
   </bookViews>
@@ -25,19 +25,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Pool Elevation (feet)</t>
   </si>
   <si>
     <t>Tube capacity (cfs)</t>
   </si>
+  <si>
+    <t>Tube capacity (maf/year)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,13 +77,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -83,6 +102,964 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3490</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3480</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3470</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3460</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3450</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3440</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3430</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3420</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3410</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3400</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3390</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3380</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3370</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.0_);_(* \(#,##0.0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>10.85952</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.598891520028639</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.483056639995915</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.193469439995917</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.7880473600040823</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.0930380800020547</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.282193919997944</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.4134323199979439</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.3709183999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.0967347199979436</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.4750464000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.3166975999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.1583488</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D635-43DC-82DC-400C436CBF2C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="841784592"/>
+        <c:axId val="842477552"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="841784592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="842477552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="842477552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="841784592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD10E4C1-4071-478B-885B-940D38BBE49B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,143 +1359,213 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2440E2B-37AB-4A2D-8A34-D830A08CF95B}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3370</v>
+        <v>3711</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>3750</v>
+      </c>
+      <c r="C2" s="1">
+        <f>B2*723.968/1000000*4</f>
+        <v>10.85952</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3380</v>
+        <v>3500</v>
       </c>
       <c r="B3">
-        <v>400</v>
+        <v>3750</v>
+      </c>
+      <c r="C3" s="1">
+        <f>B3*723.968/1000000*4</f>
+        <v>10.85952</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3390</v>
+        <v>3490</v>
       </c>
       <c r="B4">
-        <v>800</v>
+        <v>3660.0000000098898</v>
+      </c>
+      <c r="C4" s="1">
+        <f>B4*723.968/1000000*4</f>
+        <v>10.598891520028639</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3400</v>
+        <v>3480</v>
       </c>
       <c r="B5">
-        <v>1200</v>
+        <v>3619.9999999985898</v>
+      </c>
+      <c r="C5" s="1">
+        <f>B5*723.968/1000000*4</f>
+        <v>10.483056639995915</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3410</v>
+        <v>3470</v>
       </c>
       <c r="B6">
-        <v>1759.9999999992899</v>
+        <v>3519.9999999985898</v>
+      </c>
+      <c r="C6" s="1">
+        <f>B6*723.968/1000000*4</f>
+        <v>10.193469439995917</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3420</v>
+        <v>3460</v>
       </c>
       <c r="B7">
-        <v>2200</v>
+        <v>3380.0000000014102</v>
+      </c>
+      <c r="C7" s="1">
+        <f>B7*723.968/1000000*4</f>
+        <v>9.7880473600040823</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3430</v>
+        <v>3450</v>
       </c>
       <c r="B8">
-        <v>2559.9999999992901</v>
+        <v>3140.0000000007099</v>
+      </c>
+      <c r="C8" s="1">
+        <f>B8*723.968/1000000*4</f>
+        <v>9.0930380800020547</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3440</v>
       </c>
       <c r="B9">
         <v>2859.9999999992901</v>
       </c>
+      <c r="C9" s="1">
+        <f>B9*723.968/1000000*4</f>
+        <v>8.282193919997944</v>
+      </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3450</v>
+        <v>3430</v>
       </c>
       <c r="B10">
-        <v>3140.0000000007099</v>
+        <v>2559.9999999992901</v>
+      </c>
+      <c r="C10" s="1">
+        <f>B10*723.968/1000000*4</f>
+        <v>7.4134323199979439</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>3460</v>
+        <v>3420</v>
       </c>
       <c r="B11">
-        <v>3380.0000000014102</v>
+        <v>2200</v>
+      </c>
+      <c r="C11" s="1">
+        <f>B11*723.968/1000000*4</f>
+        <v>6.3709183999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>3470</v>
+        <v>3410</v>
       </c>
       <c r="B12">
-        <v>3519.9999999985898</v>
+        <v>1759.9999999992899</v>
+      </c>
+      <c r="C12" s="1">
+        <f>B12*723.968/1000000*4</f>
+        <v>5.0967347199979436</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>3480</v>
+        <v>3400</v>
       </c>
       <c r="B13">
-        <v>3619.9999999985898</v>
+        <v>1200</v>
+      </c>
+      <c r="C13" s="1">
+        <f>B13*723.968/1000000*4</f>
+        <v>3.4750464000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>3490</v>
+        <v>3390</v>
       </c>
       <c r="B14">
-        <v>3660.0000000098898</v>
+        <v>800</v>
+      </c>
+      <c r="C14" s="1">
+        <f>B14*723.968/1000000*4</f>
+        <v>2.3166975999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>3500</v>
+        <v>3380</v>
       </c>
       <c r="B15">
-        <v>3750</v>
+        <v>400</v>
+      </c>
+      <c r="C15" s="1">
+        <f>B15*723.968/1000000*4</f>
+        <v>1.1583488</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>3711</v>
+        <v>3370</v>
       </c>
       <c r="B16">
-        <v>3750</v>
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <f>B16*723.968/1000000*4</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:C16">
+    <sortCondition descending="1" ref="A2:A16"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>